<commit_message>
added get_demolition_share method to TEK/Buildings
</commit_message>
<xml_diff>
--- a/input/TEK_parameters.xlsx
+++ b/input/TEK_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Brukere-felles\lfep\EBM\task_836\Energibruksmodell\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63144FE-5BB6-4800-9C4A-6BF489A3C7B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D67921D-5BEA-4C47-95B6-38AC78C2211D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,12 +456,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B03D8-908D-4A3A-99BA-6E1BE1F7D81E}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated TEK_parameters.xlsx with period years, and added remaining get_shares per condition methods in TEK and Buildings class.
</commit_message>
<xml_diff>
--- a/input/TEK_parameters.xlsx
+++ b/input/TEK_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Brukere-felles\lfep\EBM\task_836\Energibruksmodell\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C731C91D-55E5-4D5B-9EA3-2C3C157F3477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C159A19-BBE0-45FA-8E25-B7F8F701BA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32070" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TEK_ID</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>TEK69_3</t>
+  </si>
+  <si>
+    <t>tek_period_start_year</t>
+  </si>
+  <si>
+    <t>tek_period_end_year</t>
   </si>
 </sst>
 </file>
@@ -463,117 +469,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B03D8-908D-4A3A-99BA-6E1BE1F7D81E}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2">
         <v>1950</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1963</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1956</v>
+      </c>
+      <c r="D3">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
         <v>1976</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1971</v>
+      </c>
+      <c r="D4">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5">
         <v>1986</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1981</v>
+      </c>
+      <c r="D5">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1">
         <v>1978</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>1971</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7">
         <v>1996</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1991</v>
+      </c>
+      <c r="D7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8">
         <v>2006</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2001</v>
+      </c>
+      <c r="D8">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9">
         <v>2012</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2011</v>
+      </c>
+      <c r="D9">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10">
         <v>2018</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2014</v>
+      </c>
+      <c r="D10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11">
         <v>2025</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2021</v>
+      </c>
+      <c r="D11">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12">
         <v>2030</v>
+      </c>
+      <c r="C12">
+        <v>2025</v>
+      </c>
+      <c r="D12">
+        <v>2040</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>